<commit_message>
update to published CDA FHIR logical model with patches #241
</commit_message>
<xml_diff>
--- a/docs/cda-logical-model/CodeSystem-BinaryDataEncoding.xlsx
+++ b/docs/cda-logical-model/CodeSystem-BinaryDataEncoding.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0-sd-202312-matchbox-patch</t>
+    <t>2.0.0-sd-202406-matchbox-patch</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-12T18:28:21+01:00</t>
+    <t>2024-06-19T17:47:42+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,7 +72,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>No display for ContactDetail</t>
+    <t>HL7 International - Structured Documents (http://www.hl7.org/Special/committees/structure, structdog@lists.HL7.org)</t>
   </si>
   <si>
     <t>Description</t>

</xml_diff>